<commit_message>
rad and conv maybe  success
</commit_message>
<xml_diff>
--- a/Numerical_solution.xlsx
+++ b/Numerical_solution.xlsx
@@ -423,802 +423,802 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>73.16334322299707</v>
+        <v>8.080543885060251</v>
       </c>
       <c r="B1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>79.89109494589474</v>
+        <v>9.531152088763804</v>
       </c>
       <c r="B2" t="n">
-        <v>2.97</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>78.18600372730185</v>
+        <v>10.83062920353359</v>
       </c>
       <c r="B3" t="n">
-        <v>2.94</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>72.19744905051562</v>
+        <v>11.95696150157266</v>
       </c>
       <c r="B4" t="n">
-        <v>2.91</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>64.62714950944428</v>
+        <v>12.89714609559093</v>
       </c>
       <c r="B5" t="n">
-        <v>2.88</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>57.072031700146</v>
+        <v>13.64629688757242</v>
       </c>
       <c r="B6" t="n">
-        <v>2.85</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>50.34401551419393</v>
+        <v>14.20678476527416</v>
       </c>
       <c r="B7" t="n">
-        <v>2.82</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>44.74080703092386</v>
+        <v>14.58727183400788</v>
       </c>
       <c r="B8" t="n">
-        <v>2.79</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>40.2569897868625</v>
+        <v>14.8015723540492</v>
       </c>
       <c r="B9" t="n">
-        <v>2.76</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>36.73569855890997</v>
+        <v>14.86735810086736</v>
       </c>
       <c r="B10" t="n">
-        <v>2.73</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>33.96815458284902</v>
+        <v>14.80478810667</v>
       </c>
       <c r="B11" t="n">
-        <v>2.7</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>31.75181540504508</v>
+        <v>14.63516870105605</v>
       </c>
       <c r="B12" t="n">
-        <v>2.67</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>29.9186189415928</v>
+        <v>14.37974375854355</v>
       </c>
       <c r="B13" t="n">
-        <v>2.64</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>28.34369517667977</v>
+        <v>14.05868948625613</v>
       </c>
       <c r="B14" t="n">
-        <v>2.61</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>26.94285367687633</v>
+        <v>13.69035535874627</v>
       </c>
       <c r="B15" t="n">
-        <v>2.58</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>25.66482698635673</v>
+        <v>13.29076158570177</v>
       </c>
       <c r="B16" t="n">
-        <v>2.55</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>24.48212015689398</v>
+        <v>12.87333832563655</v>
       </c>
       <c r="B17" t="n">
-        <v>2.52</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>23.38262098207372</v>
+        <v>12.4488742937919</v>
       </c>
       <c r="B18" t="n">
-        <v>2.49</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>22.36292543869286</v>
+        <v>12.02563229109575</v>
       </c>
       <c r="B19" t="n">
-        <v>2.46</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>21.42358014546346</v>
+        <v>11.60958549242395</v>
       </c>
       <c r="B20" t="n">
-        <v>2.43</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20.56603859723236</v>
+        <v>11.20472970985736</v>
       </c>
       <c r="B21" t="n">
-        <v>2.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>19.79096128327427</v>
+        <v>10.81343182559095</v>
       </c>
       <c r="B22" t="n">
-        <v>2.37</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>19.09746691622519</v>
+        <v>10.43678176047183</v>
       </c>
       <c r="B23" t="n">
-        <v>2.34</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>18.48299242668458</v>
+        <v>10.07492346136092</v>
       </c>
       <c r="B24" t="n">
-        <v>2.31</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>17.9434969750838</v>
+        <v>9.727348445220457</v>
       </c>
       <c r="B25" t="n">
-        <v>2.28</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>17.47382360199219</v>
+        <v>9.393142699491136</v>
       </c>
       <c r="B26" t="n">
-        <v>2.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>17.06809874231089</v>
+        <v>9.071183757189772</v>
       </c>
       <c r="B27" t="n">
-        <v>2.22</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>16.72010067800028</v>
+        <v>8.760289343370744</v>
       </c>
       <c r="B28" t="n">
-        <v>2.19</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>16.4235636837854</v>
+        <v>8.459322130556529</v>
       </c>
       <c r="B29" t="n">
-        <v>2.16</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>16.1724077011603</v>
+        <v>8.167256989271493</v>
       </c>
       <c r="B30" t="n">
-        <v>2.13</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>15.96089692691908</v>
+        <v>7.88321790317741</v>
       </c>
       <c r="B31" t="n">
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>15.78373755743411</v>
+        <v>7.60649169614851</v>
       </c>
       <c r="B32" t="n">
-        <v>2.07</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>15.63612740373543</v>
+        <v>7.336525144955772</v>
       </c>
       <c r="B33" t="n">
-        <v>2.04</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>15.51376993352716</v>
+        <v>7.072911150032667</v>
       </c>
       <c r="B34" t="n">
-        <v>2.01</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>15.41286374525879</v>
+        <v>6.81536858893503</v>
       </c>
       <c r="B35" t="n">
-        <v>1.98</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>15.33007636380086</v>
+        <v>6.56371941692197</v>
       </c>
       <c r="B36" t="n">
-        <v>1.95</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>15.26250907910241</v>
+        <v>6.317865596997422</v>
       </c>
       <c r="B37" t="n">
-        <v>1.92</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>15.20765761114671</v>
+        <v>6.077767590845554</v>
       </c>
       <c r="B38" t="n">
-        <v>1.89</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>15.16337180191425</v>
+        <v>5.843425445981893</v>
       </c>
       <c r="B39" t="n">
-        <v>1.86</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>15.12781633227655</v>
+        <v>5.61486297565682</v>
       </c>
       <c r="B40" t="n">
-        <v>1.83</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>15.09943360502706</v>
+        <v>5.392115135001973</v>
       </c>
       <c r="B41" t="n">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>15.07690936307438</v>
+        <v>5.175218430189148</v>
       </c>
       <c r="B42" t="n">
-        <v>1.77</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>15.05914125525123</v>
+        <v>4.964204033927899</v>
       </c>
       <c r="B43" t="n">
-        <v>1.74</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>15.04521035725577</v>
+        <v>4.759093197354787</v>
       </c>
       <c r="B44" t="n">
-        <v>1.71</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>15.0343555488721</v>
+        <v>4.559894523775483</v>
       </c>
       <c r="B45" t="n">
-        <v>1.68</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>15.0259506008714</v>
+        <v>4.366602685311591</v>
       </c>
       <c r="B46" t="n">
-        <v>1.65</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>15.0194838081772</v>
+        <v>4.1791982041957</v>
       </c>
       <c r="B47" t="n">
-        <v>1.62</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>15.01454000269536</v>
+        <v>3.997647974443112</v>
       </c>
       <c r="B48" t="n">
-        <v>1.59</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>15.0107847800694</v>
+        <v>3.821906258358013</v>
       </c>
       <c r="B49" t="n">
-        <v>1.56</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>15.00795077524089</v>
+        <v>3.651915949803083</v>
       </c>
       <c r="B50" t="n">
-        <v>1.53</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>15.00582582109013</v>
+        <v>3.487609948643751</v>
       </c>
       <c r="B51" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>15.00424282317647</v>
+        <v>3.328912536173107</v>
       </c>
       <c r="B52" t="n">
-        <v>1.47</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>15.003071182876</v>
+        <v>3.175740678855391</v>
       </c>
       <c r="B53" t="n">
-        <v>1.44</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>15.00220960219855</v>
+        <v>3.028005217392945</v>
       </c>
       <c r="B54" t="n">
-        <v>1.41</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>15.00158010697498</v>
+        <v>2.885611920554368</v>
       </c>
       <c r="B55" t="n">
-        <v>1.38</v>
+        <v>0.9199999999999999</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>15.00112313126925</v>
+        <v>2.748462399326741</v>
       </c>
       <c r="B56" t="n">
-        <v>1.35</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>15.00079351463751</v>
+        <v>2.616454887786631</v>
       </c>
       <c r="B57" t="n">
-        <v>1.32</v>
+        <v>0.8799999999999999</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>15.00055727484335</v>
+        <v>2.489484903708274</v>
       </c>
       <c r="B58" t="n">
-        <v>1.29</v>
+        <v>0.8599999999999999</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>15.00038903119247</v>
+        <v>2.367445805371631</v>
       </c>
       <c r="B59" t="n">
-        <v>1.26</v>
+        <v>0.8400000000000001</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>15.00026996714143</v>
+        <v>2.250229262057644</v>
       </c>
       <c r="B60" t="n">
-        <v>1.23</v>
+        <v>0.8200000000000001</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>15.0001862345959</v>
+        <v>2.137725655222312</v>
       </c>
       <c r="B61" t="n">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>15.00012771579418</v>
+        <v>2.029824425752395</v>
       </c>
       <c r="B62" t="n">
-        <v>1.17</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>15.00008707144195</v>
+        <v>1.926414380622248</v>
       </c>
       <c r="B63" t="n">
-        <v>1.14</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>15.00005901549139</v>
+        <v>1.827383969930622</v>
       </c>
       <c r="B64" t="n">
-        <v>1.11</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>15.00003976746308</v>
+        <v>1.732621542990557</v>
       </c>
       <c r="B65" t="n">
-        <v>1.08</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>15.0000266424272</v>
+        <v>1.642015590024698</v>
       </c>
       <c r="B66" t="n">
-        <v>1.05</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>15.00001774664463</v>
+        <v>1.555454974144084</v>
       </c>
       <c r="B67" t="n">
-        <v>1.02</v>
+        <v>0.6799999999999999</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>15.00001175351645</v>
+        <v>1.472829156724799</v>
       </c>
       <c r="B68" t="n">
-        <v>0.9900000000000002</v>
+        <v>0.6599999999999999</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>15.00000774000125</v>
+        <v>1.394028418051164</v>
       </c>
       <c r="B69" t="n">
-        <v>0.96</v>
+        <v>0.6399999999999999</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>15.00000506813791</v>
+        <v>1.318944074135572</v>
       </c>
       <c r="B70" t="n">
-        <v>0.9300000000000002</v>
+        <v>0.6199999999999999</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>15.0000032999136</v>
+        <v>1.247468689919287</v>
       </c>
       <c r="B71" t="n">
-        <v>0.8999999999999999</v>
+        <v>0.5999999999999999</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>15.0000021365658</v>
+        <v>1.179496288591565</v>
       </c>
       <c r="B72" t="n">
-        <v>0.8700000000000001</v>
+        <v>0.5800000000000001</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>15.00000137563245</v>
+        <v>1.114922556472948</v>
       </c>
       <c r="B73" t="n">
-        <v>0.8399999999999999</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>15.00000088079395</v>
+        <v>1.053645042753885</v>
       </c>
       <c r="B74" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>15.00000056084917</v>
+        <v>0.9955633533334094</v>
       </c>
       <c r="B75" t="n">
-        <v>0.7800000000000002</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>15.00000035516706</v>
+        <v>0.9405793380448131</v>
       </c>
       <c r="B76" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>15.00000022369306</v>
+        <v>0.8885972706247003</v>
       </c>
       <c r="B77" t="n">
-        <v>0.7200000000000002</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>15.00000014012767</v>
+        <v>0.8395240209014219</v>
       </c>
       <c r="B78" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>15.00000008731263</v>
+        <v>0.7932692187896464</v>
       </c>
       <c r="B79" t="n">
-        <v>0.6600000000000001</v>
+        <v>0.4399999999999999</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>15.00000005411897</v>
+        <v>0.7497454098165122</v>
       </c>
       <c r="B80" t="n">
-        <v>0.6299999999999999</v>
+        <v>0.4199999999999999</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>15.0000000333726</v>
+        <v>0.7088682020094552</v>
       </c>
       <c r="B81" t="n">
-        <v>0.6000000000000001</v>
+        <v>0.3999999999999999</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>15.0000000204779</v>
+        <v>0.6705564040814807</v>
       </c>
       <c r="B82" t="n">
-        <v>0.5700000000000003</v>
+        <v>0.3799999999999999</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>15.00000001250686</v>
+        <v>0.6347321549525304</v>
       </c>
       <c r="B83" t="n">
-        <v>0.54</v>
+        <v>0.3599999999999999</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>15.00000000760639</v>
+        <v>0.6013210447056849</v>
       </c>
       <c r="B84" t="n">
-        <v>0.5100000000000002</v>
+        <v>0.3399999999999999</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>15.00000000460938</v>
+        <v>0.5702522271432713</v>
       </c>
       <c r="B85" t="n">
-        <v>0.48</v>
+        <v>0.3200000000000001</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>15.00000000278663</v>
+        <v>0.5414585241504142</v>
       </c>
       <c r="B86" t="n">
-        <v>0.4500000000000002</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>15.00000000168347</v>
+        <v>0.5148765221131271</v>
       </c>
       <c r="B87" t="n">
-        <v>0.4199999999999999</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>15.0000000010188</v>
+        <v>0.4904466606442384</v>
       </c>
       <c r="B88" t="n">
-        <v>0.3900000000000001</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>15.00000000061993</v>
+        <v>0.4681133138921609</v>
       </c>
       <c r="B89" t="n">
-        <v>0.3600000000000003</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>15.00000000038085</v>
+        <v>0.4478248647106398</v>
       </c>
       <c r="B90" t="n">
-        <v>0.3300000000000001</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>15.00000000023783</v>
+        <v>0.429533771955505</v>
       </c>
       <c r="B91" t="n">
-        <v>0.3000000000000003</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>15.00000000015149</v>
+        <v>0.4131966311701945</v>
       </c>
       <c r="B92" t="n">
-        <v>0.27</v>
+        <v>0.1799999999999999</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>15.00000000009919</v>
+        <v>0.398774228914931</v>
       </c>
       <c r="B93" t="n">
-        <v>0.2400000000000002</v>
+        <v>0.1599999999999999</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>15.00000000006605</v>
+        <v>0.3862315909659628</v>
       </c>
       <c r="B94" t="n">
-        <v>0.21</v>
+        <v>0.1399999999999999</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>15.00000000004502</v>
+        <v>0.3755380246013829</v>
       </c>
       <c r="B95" t="n">
-        <v>0.1800000000000002</v>
+        <v>0.1199999999999999</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>15.00000000003246</v>
+        <v>0.3666671551686136</v>
       </c>
       <c r="B96" t="n">
-        <v>0.1499999999999999</v>
+        <v>0.09999999999999987</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>15.00000000002302</v>
+        <v>0.3595969571013597</v>
       </c>
       <c r="B97" t="n">
-        <v>0.1200000000000001</v>
+        <v>0.08000000000000007</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>15.00000000001779</v>
+        <v>0.3543097795372319</v>
       </c>
       <c r="B98" t="n">
-        <v>0.0900000000000003</v>
+        <v>0.06000000000000005</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>15.00000000001376</v>
+        <v>0.3507923666626311</v>
       </c>
       <c r="B99" t="n">
-        <v>0.06000000000000005</v>
+        <v>0.04000000000000004</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>15.0000000000116</v>
+        <v>0.3490358728799947</v>
       </c>
       <c r="B100" t="n">
-        <v>0.03000000000000025</v>
+        <v>0.02000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rad and conv vs lrs success
</commit_message>
<xml_diff>
--- a/Numerical_solution.xlsx
+++ b/Numerical_solution.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,802 +423,2002 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>8.080543885060251</v>
+        <v>30.52048042809639</v>
       </c>
       <c r="B1" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9.531152088763804</v>
+        <v>30.35308049931223</v>
       </c>
       <c r="B2" t="n">
-        <v>1.98</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>10.83062920353359</v>
+        <v>29.90191631399938</v>
       </c>
       <c r="B3" t="n">
-        <v>1.96</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>11.95696150157266</v>
+        <v>29.22462627027886</v>
       </c>
       <c r="B4" t="n">
-        <v>1.94</v>
+        <v>2.47</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>12.89714609559093</v>
+        <v>28.37202449597146</v>
       </c>
       <c r="B5" t="n">
-        <v>1.92</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>13.64629688757242</v>
+        <v>27.38856153384535</v>
       </c>
       <c r="B6" t="n">
-        <v>1.9</v>
+        <v>2.45</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>14.20678476527416</v>
+        <v>26.31280213332121</v>
       </c>
       <c r="B7" t="n">
-        <v>1.88</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>14.58727183400788</v>
+        <v>25.17791407524845</v>
       </c>
       <c r="B8" t="n">
-        <v>1.86</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>14.8015723540492</v>
+        <v>24.01216196277664</v>
       </c>
       <c r="B9" t="n">
-        <v>1.84</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>14.86735810086736</v>
+        <v>22.83940018718897</v>
       </c>
       <c r="B10" t="n">
-        <v>1.82</v>
+        <v>2.41</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>14.80478810667</v>
+        <v>21.80843089029867</v>
       </c>
       <c r="B11" t="n">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>14.63516870105605</v>
+        <v>20.92777861174693</v>
       </c>
       <c r="B12" t="n">
-        <v>1.78</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>14.37974375854355</v>
+        <v>20.07670581973173</v>
       </c>
       <c r="B13" t="n">
-        <v>1.76</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>14.05868948625613</v>
+        <v>19.26171649713979</v>
       </c>
       <c r="B14" t="n">
-        <v>1.74</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>13.69035535874627</v>
+        <v>18.48788347681841</v>
       </c>
       <c r="B15" t="n">
-        <v>1.72</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>13.29076158570177</v>
+        <v>17.75903640625575</v>
       </c>
       <c r="B16" t="n">
-        <v>1.7</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>12.87333832563655</v>
+        <v>17.07793852534849</v>
       </c>
       <c r="B17" t="n">
-        <v>1.68</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>12.4488742937919</v>
+        <v>16.44645178985769</v>
       </c>
       <c r="B18" t="n">
-        <v>1.66</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>12.02563229109575</v>
+        <v>15.86569004122862</v>
       </c>
       <c r="B19" t="n">
-        <v>1.64</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>11.60958549242395</v>
+        <v>15.33616007135112</v>
       </c>
       <c r="B20" t="n">
-        <v>1.62</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>11.20472970985736</v>
+        <v>14.85789055747222</v>
       </c>
       <c r="B21" t="n">
-        <v>1.6</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>10.81343182559095</v>
+        <v>14.43054894758546</v>
       </c>
       <c r="B22" t="n">
-        <v>1.58</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>10.43678176047183</v>
+        <v>14.05354646017838</v>
       </c>
       <c r="B23" t="n">
-        <v>1.56</v>
+        <v>2.28</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>10.07492346136092</v>
+        <v>13.72613142467986</v>
       </c>
       <c r="B24" t="n">
-        <v>1.54</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>9.727348445220457</v>
+        <v>13.44747123117486</v>
       </c>
       <c r="B25" t="n">
-        <v>1.52</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>9.393142699491136</v>
+        <v>13.21672318097467</v>
       </c>
       <c r="B26" t="n">
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>9.071183757189772</v>
+        <v>13.03309453495649</v>
       </c>
       <c r="B27" t="n">
-        <v>1.48</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>8.760289343370744</v>
+        <v>12.89589204578596</v>
       </c>
       <c r="B28" t="n">
-        <v>1.46</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>8.459322130556529</v>
+        <v>12.80456123514364</v>
       </c>
       <c r="B29" t="n">
-        <v>1.44</v>
+        <v>2.22</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>8.167256989271493</v>
+        <v>12.75871563993428</v>
       </c>
       <c r="B30" t="n">
-        <v>1.42</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>7.88321790317741</v>
+        <v>0.1711368974018228</v>
       </c>
       <c r="B31" t="n">
-        <v>1.4</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>7.60649169614851</v>
+        <v>0.0007020358289082651</v>
       </c>
       <c r="B32" t="n">
-        <v>1.38</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>7.336525144955772</v>
+        <v>1.992550267004844e-06</v>
       </c>
       <c r="B33" t="n">
-        <v>1.36</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>7.072911150032667</v>
+        <v>4.641321993403835e-09</v>
       </c>
       <c r="B34" t="n">
-        <v>1.34</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>6.81536858893503</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B35" t="n">
-        <v>1.32</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>6.56371941692197</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B36" t="n">
-        <v>1.3</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>6.317865596997422</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B37" t="n">
-        <v>1.28</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>6.077767590845554</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B38" t="n">
-        <v>1.26</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>5.843425445981893</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B39" t="n">
-        <v>1.24</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>5.61486297565682</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B40" t="n">
-        <v>1.22</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>5.392115135001973</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B41" t="n">
-        <v>1.2</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>5.175218430189148</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B42" t="n">
-        <v>1.18</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>4.964204033927899</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B43" t="n">
-        <v>1.16</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>4.759093197354787</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B44" t="n">
-        <v>1.14</v>
+        <v>2.07</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>4.559894523775483</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B45" t="n">
-        <v>1.12</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>4.366602685311591</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B46" t="n">
-        <v>1.1</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>4.1791982041957</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B47" t="n">
-        <v>1.08</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>3.997647974443112</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B48" t="n">
-        <v>1.06</v>
+        <v>2.03</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>3.821906258358013</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B49" t="n">
-        <v>1.04</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>3.651915949803083</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B50" t="n">
-        <v>1.02</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>3.487609948643751</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>3.328912536173107</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B52" t="n">
-        <v>0.98</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>3.175740678855391</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B53" t="n">
-        <v>0.96</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>3.028005217392945</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B54" t="n">
-        <v>0.9399999999999999</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2.885611920554368</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B55" t="n">
-        <v>0.9199999999999999</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2.748462399326741</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B56" t="n">
-        <v>0.8999999999999999</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2.616454887786631</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B57" t="n">
-        <v>0.8799999999999999</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2.489484903708274</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B58" t="n">
-        <v>0.8599999999999999</v>
+        <v>1.93</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2.367445805371631</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B59" t="n">
-        <v>0.8400000000000001</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2.250229262057644</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B60" t="n">
-        <v>0.8200000000000001</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2.137725655222312</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B61" t="n">
-        <v>0.8</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2.029824425752395</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B62" t="n">
-        <v>0.78</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1.926414380622248</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B63" t="n">
-        <v>0.76</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1.827383969930622</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B64" t="n">
-        <v>0.74</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>1.732621542990557</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B65" t="n">
-        <v>0.72</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1.642015590024698</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B66" t="n">
-        <v>0.7</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1.555454974144084</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B67" t="n">
-        <v>0.6799999999999999</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1.472829156724799</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B68" t="n">
-        <v>0.6599999999999999</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1.394028418051164</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B69" t="n">
-        <v>0.6399999999999999</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1.318944074135572</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B70" t="n">
-        <v>0.6199999999999999</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1.247468689919287</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B71" t="n">
-        <v>0.5999999999999999</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1.179496288591565</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B72" t="n">
-        <v>0.5800000000000001</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>1.114922556472948</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B73" t="n">
-        <v>0.5600000000000001</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1.053645042753885</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B74" t="n">
-        <v>0.54</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0.9955633533334094</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B75" t="n">
-        <v>0.52</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>0.9405793380448131</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B76" t="n">
-        <v>0.5</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0.8885972706247003</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B77" t="n">
-        <v>0.48</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>0.8395240209014219</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B78" t="n">
-        <v>0.46</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>0.7932692187896464</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B79" t="n">
-        <v>0.4399999999999999</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0.7497454098165122</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B80" t="n">
-        <v>0.4199999999999999</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0.7088682020094552</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B81" t="n">
-        <v>0.3999999999999999</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>0.6705564040814807</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B82" t="n">
-        <v>0.3799999999999999</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>0.6347321549525304</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B83" t="n">
-        <v>0.3599999999999999</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>0.6013210447056849</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B84" t="n">
-        <v>0.3399999999999999</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>0.5702522271432713</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B85" t="n">
-        <v>0.3200000000000001</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>0.5414585241504142</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B86" t="n">
-        <v>0.3</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0.5148765221131271</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B87" t="n">
-        <v>0.28</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>0.4904466606442384</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B88" t="n">
-        <v>0.26</v>
+        <v>1.63</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0.4681133138921609</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B89" t="n">
-        <v>0.24</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>0.4478248647106398</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B90" t="n">
-        <v>0.22</v>
+        <v>1.61</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>0.429533771955505</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B91" t="n">
-        <v>0.2</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>0.4131966311701945</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B92" t="n">
-        <v>0.1799999999999999</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>0.398774228914931</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B93" t="n">
-        <v>0.1599999999999999</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0.3862315909659628</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B94" t="n">
-        <v>0.1399999999999999</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>0.3755380246013829</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B95" t="n">
-        <v>0.1199999999999999</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>0.3666671551686136</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B96" t="n">
-        <v>0.09999999999999987</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>0.3595969571013597</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B97" t="n">
-        <v>0.08000000000000007</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0.3543097795372319</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B98" t="n">
-        <v>0.06000000000000005</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0.3507923666626311</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B99" t="n">
-        <v>0.04000000000000004</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>0.3490358728799947</v>
+        <v>3.515197022352368e-10</v>
       </c>
       <c r="B100" t="n">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B101" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B102" t="n">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B103" t="n">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B104" t="n">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B105" t="n">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B106" t="n">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B107" t="n">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B108" t="n">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B109" t="n">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B110" t="n">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B111" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B112" t="n">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B113" t="n">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B114" t="n">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B115" t="n">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B116" t="n">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B117" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B118" t="n">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B119" t="n">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B120" t="n">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B121" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B122" t="n">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B123" t="n">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B124" t="n">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B125" t="n">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B126" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B127" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B128" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B129" t="n">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B130" t="n">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B131" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B132" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B133" t="n">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B134" t="n">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B135" t="n">
+        <v>1.16</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B136" t="n">
+        <v>1.15</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B137" t="n">
+        <v>1.14</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B138" t="n">
+        <v>1.13</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B139" t="n">
+        <v>1.12</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B140" t="n">
+        <v>1.11</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B141" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B142" t="n">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B143" t="n">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B144" t="n">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B145" t="n">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B146" t="n">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B147" t="n">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>3.515197022352368e-10</v>
+      </c>
+      <c r="B148" t="n">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>-6.821210263296962e-13</v>
+      </c>
+      <c r="B149" t="n">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>-6.821210263296962e-13</v>
+      </c>
+      <c r="B150" t="n">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>0</v>
+      </c>
+      <c r="B151" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>-5.684341886080801e-14</v>
+      </c>
+      <c r="B152" t="n">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>-4.547473508864641e-13</v>
+      </c>
+      <c r="B153" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>-1.70530256582424e-13</v>
+      </c>
+      <c r="B154" t="n">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>-2.273736754432321e-13</v>
+      </c>
+      <c r="B155" t="n">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>0</v>
+      </c>
+      <c r="B156" t="n">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>0</v>
+      </c>
+      <c r="B157" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>0</v>
+      </c>
+      <c r="B158" t="n">
+        <v>0.9299999999999999</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>0</v>
+      </c>
+      <c r="B159" t="n">
+        <v>0.9199999999999999</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>-5.684341886080801e-14</v>
+      </c>
+      <c r="B160" t="n">
+        <v>0.9099999999999999</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>0</v>
+      </c>
+      <c r="B161" t="n">
+        <v>0.8999999999999999</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>0</v>
+      </c>
+      <c r="B162" t="n">
+        <v>0.8899999999999999</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>0</v>
+      </c>
+      <c r="B163" t="n">
+        <v>0.8799999999999999</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>0</v>
+      </c>
+      <c r="B164" t="n">
+        <v>0.8699999999999999</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>0</v>
+      </c>
+      <c r="B165" t="n">
+        <v>0.8599999999999999</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>0</v>
+      </c>
+      <c r="B166" t="n">
+        <v>0.8499999999999999</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>0</v>
+      </c>
+      <c r="B167" t="n">
+        <v>0.8399999999999999</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>0</v>
+      </c>
+      <c r="B168" t="n">
+        <v>0.8300000000000001</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>0</v>
+      </c>
+      <c r="B169" t="n">
+        <v>0.8200000000000001</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>0</v>
+      </c>
+      <c r="B170" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>0</v>
+      </c>
+      <c r="B171" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>0</v>
+      </c>
+      <c r="B172" t="n">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>0</v>
+      </c>
+      <c r="B173" t="n">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>0</v>
+      </c>
+      <c r="B174" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>0</v>
+      </c>
+      <c r="B175" t="n">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>0</v>
+      </c>
+      <c r="B176" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>0</v>
+      </c>
+      <c r="B177" t="n">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>0</v>
+      </c>
+      <c r="B178" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>0</v>
+      </c>
+      <c r="B179" t="n">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>0</v>
+      </c>
+      <c r="B180" t="n">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>0</v>
+      </c>
+      <c r="B181" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>0</v>
+      </c>
+      <c r="B182" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>0</v>
+      </c>
+      <c r="B183" t="n">
+        <v>0.6799999999999999</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>0</v>
+      </c>
+      <c r="B184" t="n">
+        <v>0.6699999999999999</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>0</v>
+      </c>
+      <c r="B185" t="n">
+        <v>0.6599999999999999</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>0</v>
+      </c>
+      <c r="B186" t="n">
+        <v>0.6499999999999999</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>0</v>
+      </c>
+      <c r="B187" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>0</v>
+      </c>
+      <c r="B188" t="n">
+        <v>0.6299999999999999</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>0</v>
+      </c>
+      <c r="B189" t="n">
+        <v>0.6199999999999999</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>0</v>
+      </c>
+      <c r="B190" t="n">
+        <v>0.6099999999999999</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>0</v>
+      </c>
+      <c r="B191" t="n">
+        <v>0.5999999999999999</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>0</v>
+      </c>
+      <c r="B192" t="n">
+        <v>0.5899999999999999</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>0</v>
+      </c>
+      <c r="B193" t="n">
+        <v>0.5800000000000001</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>0</v>
+      </c>
+      <c r="B194" t="n">
+        <v>0.5700000000000001</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>0</v>
+      </c>
+      <c r="B195" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>0</v>
+      </c>
+      <c r="B196" t="n">
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>0</v>
+      </c>
+      <c r="B197" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>0</v>
+      </c>
+      <c r="B198" t="n">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>0</v>
+      </c>
+      <c r="B199" t="n">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>0</v>
+      </c>
+      <c r="B200" t="n">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>0</v>
+      </c>
+      <c r="B201" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>0</v>
+      </c>
+      <c r="B202" t="n">
+        <v>0.4899999999999998</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>0</v>
+      </c>
+      <c r="B203" t="n">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>0</v>
+      </c>
+      <c r="B204" t="n">
+        <v>0.4699999999999998</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>0</v>
+      </c>
+      <c r="B205" t="n">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>0</v>
+      </c>
+      <c r="B206" t="n">
+        <v>0.4500000000000002</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>0</v>
+      </c>
+      <c r="B207" t="n">
+        <v>0.4399999999999999</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>0</v>
+      </c>
+      <c r="B208" t="n">
+        <v>0.4300000000000002</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>0</v>
+      </c>
+      <c r="B209" t="n">
+        <v>0.4199999999999999</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>0</v>
+      </c>
+      <c r="B210" t="n">
+        <v>0.4100000000000001</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>0</v>
+      </c>
+      <c r="B211" t="n">
+        <v>0.3999999999999999</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>0</v>
+      </c>
+      <c r="B212" t="n">
+        <v>0.3900000000000001</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>0</v>
+      </c>
+      <c r="B213" t="n">
+        <v>0.3799999999999999</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>0</v>
+      </c>
+      <c r="B214" t="n">
+        <v>0.3700000000000001</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>0</v>
+      </c>
+      <c r="B215" t="n">
+        <v>0.3599999999999999</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>0</v>
+      </c>
+      <c r="B216" t="n">
+        <v>0.3500000000000001</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>0</v>
+      </c>
+      <c r="B217" t="n">
+        <v>0.3399999999999999</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>0</v>
+      </c>
+      <c r="B218" t="n">
+        <v>0.3300000000000001</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>0</v>
+      </c>
+      <c r="B219" t="n">
+        <v>0.3199999999999998</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>0</v>
+      </c>
+      <c r="B220" t="n">
+        <v>0.3100000000000001</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>0</v>
+      </c>
+      <c r="B221" t="n">
+        <v>0.2999999999999998</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>0</v>
+      </c>
+      <c r="B222" t="n">
+        <v>0.29</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>0</v>
+      </c>
+      <c r="B223" t="n">
+        <v>0.2799999999999998</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>0</v>
+      </c>
+      <c r="B224" t="n">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>0</v>
+      </c>
+      <c r="B225" t="n">
+        <v>0.2599999999999998</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>0</v>
+      </c>
+      <c r="B226" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>0</v>
+      </c>
+      <c r="B227" t="n">
+        <v>0.2399999999999998</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>0</v>
+      </c>
+      <c r="B228" t="n">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>0</v>
+      </c>
+      <c r="B229" t="n">
+        <v>0.2199999999999998</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>0</v>
+      </c>
+      <c r="B230" t="n">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>0</v>
+      </c>
+      <c r="B231" t="n">
+        <v>0.1999999999999997</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>1.13686837721616e-13</v>
+      </c>
+      <c r="B232" t="n">
+        <v>0.1899999999999999</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>2.273736754432321e-13</v>
+      </c>
+      <c r="B233" t="n">
+        <v>0.1800000000000002</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>1.13686837721616e-13</v>
+      </c>
+      <c r="B234" t="n">
+        <v>0.1699999999999999</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>1.13686837721616e-13</v>
+      </c>
+      <c r="B235" t="n">
+        <v>0.1600000000000001</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>-2.842170943040401e-13</v>
+      </c>
+      <c r="B236" t="n">
+        <v>0.1499999999999999</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>0</v>
+      </c>
+      <c r="B237" t="n">
+        <v>0.1400000000000001</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>-5.684341886080801e-14</v>
+      </c>
+      <c r="B238" t="n">
+        <v>0.1299999999999999</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>-5.684341886080801e-14</v>
+      </c>
+      <c r="B239" t="n">
+        <v>0.1200000000000001</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>0</v>
+      </c>
+      <c r="B240" t="n">
+        <v>0.1099999999999999</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>1.13686837721616e-13</v>
+      </c>
+      <c r="B241" t="n">
+        <v>0.1000000000000001</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>3.410605131648481e-13</v>
+      </c>
+      <c r="B242" t="n">
+        <v>0.08999999999999986</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>6.821210263296962e-13</v>
+      </c>
+      <c r="B243" t="n">
+        <v>0.08000000000000007</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>7.389644451905042e-13</v>
+      </c>
+      <c r="B244" t="n">
+        <v>0.06999999999999984</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>6.821210263296962e-13</v>
+      </c>
+      <c r="B245" t="n">
+        <v>0.06000000000000005</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>5.115907697472721e-13</v>
+      </c>
+      <c r="B246" t="n">
+        <v>0.04999999999999982</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>2.842170943040401e-13</v>
+      </c>
+      <c r="B247" t="n">
+        <v>0.04000000000000004</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>1.13686837721616e-13</v>
+      </c>
+      <c r="B248" t="n">
+        <v>0.0299999999999998</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>2.842170943040401e-13</v>
+      </c>
+      <c r="B249" t="n">
         <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>3.410605131648481e-13</v>
+      </c>
+      <c r="B250" t="n">
+        <v>0.009999999999999787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>